<commit_message>
Auto export testcases (1 scénářů)
</commit_message>
<xml_diff>
--- a/vystup.xlsx
+++ b/vystup.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -488,12 +488,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -513,12 +513,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -538,12 +538,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -563,12 +563,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -588,12 +588,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -613,12 +613,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -638,12 +638,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -663,12 +663,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -688,12 +688,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -713,12 +713,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -738,12 +738,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -763,12 +763,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -788,12 +788,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -813,12 +813,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -838,12 +838,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -863,12 +863,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -888,12 +888,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -913,12 +913,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -938,12 +938,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -963,12 +963,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -988,12 +988,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1013,12 +1013,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TC_VASaktivace_b2c_vasaktivace_aktivuj_fwa_bi_s_rentalem</t>
+          <t>(003)_b2c_dsl_vasaktivate_aktivuj dsl + rental + security na b2c</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VASaktivace</t>
+          <t>vasaktivate</t>
         </is>
       </c>
       <c r="C24" t="n">

</xml_diff>